<commit_message>
Fix NIP wrong format in AdminExport
</commit_message>
<xml_diff>
--- a/public/file/Book1.xlsx
+++ b/public/file/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A\Project\Sec\dispress\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7F2305-D69C-4B6D-9965-B62BBA25D2D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61FA8B9-7D47-4FDD-A592-85A20F362BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3F00758C-3CCA-4504-98DA-D1AB7AE974C6}"/>
   </bookViews>
@@ -423,12 +423,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -439,7 +439,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -465,7 +465,6 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
     </row>

</xml_diff>

<commit_message>
added data validation to jabatan and level
</commit_message>
<xml_diff>
--- a/public/file/Book1.xlsx
+++ b/public/file/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A\Project\Sec\dispress\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61FA8B9-7D47-4FDD-A592-85A20F362BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0486557-BA19-4DC8-9F88-091E4C7119D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3F00758C-3CCA-4504-98DA-D1AB7AE974C6}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +469,14 @@
       <c r="G2" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Jabatan" prompt="Harap inputkan jabatan" sqref="D2:D1048576" xr:uid="{66FD9E86-1041-4351-9B6E-5CA9BBBCF412}">
+      <formula1>"kepala sekolah,wakil kepala sekolah,kurikulum,kesiswaan,sarana dan prasarana,kepala jurusan,hubin,bimbingan konseling,guru umum,tata usaha"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Level" prompt="Harap pilih level yang sesuai_x000a_" sqref="C2:C1048576" xr:uid="{8D83EC4B-8E28-41A8-8C38-398A8EF9DBC5}">
+      <formula1>"admin,officer,staff"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>